<commit_message>
merged provincial, city, region fields; ready to test on new converted pdfs
</commit_message>
<xml_diff>
--- a/DOH/datafile_input.xlsx
+++ b/DOH/datafile_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jomelle Wong\GitHub\workstuff\DOH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631B9517-B205-41D0-BE59-33AA20BA62E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E243D418-7AF2-4084-B658-5CBD595A65C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9820" yWindow="2780" windowWidth="28510" windowHeight="18030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="70" yWindow="13670" windowWidth="20990" windowHeight="7140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -1058,7 +1058,8 @@
   <dimension ref="A1:M202"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>

</xml_diff>